<commit_message>
fixed incorrect nutrition facts and typos
</commit_message>
<xml_diff>
--- a/nutrition-calcs/breakfast-burritos.xlsx
+++ b/nutrition-calcs/breakfast-burritos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">TOTAL</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avocado oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.dillons.com/p/simple-truth-organic-refined-avocado-oil-bottle/0001111003441</t>
   </si>
   <si>
     <t xml:space="preserve">russet potato</t>
@@ -101,6 +107,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,12 +129,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,36 +181,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -222,311 +239,336 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="95.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="95.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <f aca="false">14*3</f>
+        <v>42</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>37</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C4" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D4" s="6" t="n">
         <v>1.9</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E4" s="6" t="n">
         <v>0.2</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F4" s="6" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <f aca="false">0*12</f>
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C5" s="6" t="n">
         <f aca="false">0*12</f>
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D5" s="6" t="n">
         <f aca="false">0*12</f>
         <v>0</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E5" s="6" t="n">
         <f aca="false">5*12</f>
         <v>60</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F5" s="6" t="n">
         <f aca="false">6*12</f>
         <v>72</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="n">
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="n">
+      <c r="C6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <f aca="false">2*(8/3)</f>
         <v>5.33333333333333</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C7" s="6" t="n">
         <f aca="false">0*(8/3)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">1*(8/3)</f>
         <v>2.66666666666667</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E7" s="6" t="n">
         <f aca="false">13*(8/3)</f>
         <v>34.6666666666667</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F7" s="6" t="n">
         <f aca="false">10*(8/3)</f>
         <v>26.6666666666667</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="n">
+      <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <f aca="false">31*8</f>
         <v>248</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C8" s="6" t="n">
         <f aca="false">23*8</f>
         <v>184</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">0*120*12</f>
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E8" s="6" t="n">
         <f aca="false">4*12</f>
         <v>48</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F8" s="6" t="n">
         <f aca="false">8*12</f>
         <v>96</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="n">
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="n">
         <f aca="false">8*1</f>
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C9" s="6" t="n">
         <f aca="false">0*0</f>
         <v>0</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D9" s="6" t="n">
         <f aca="false">0*0</f>
         <v>0</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E9" s="6" t="n">
         <f aca="false">9*8</f>
         <v>72</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F9" s="6" t="n">
         <f aca="false">6*8</f>
         <v>48</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <f aca="false">SUM(B3:B8)</f>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <f aca="false">SUM(B3:B9)</f>
         <v>299.333333333333</v>
       </c>
-      <c r="C10" s="3" t="n">
-        <f aca="false">SUM(C3:C8)</f>
+      <c r="C11" s="6" t="n">
+        <f aca="false">SUM(C3:C9)</f>
         <v>188</v>
       </c>
-      <c r="D10" s="3" t="n">
-        <f aca="false">SUM(D3:D8)</f>
+      <c r="D11" s="6" t="n">
+        <f aca="false">SUM(D3:D9)</f>
         <v>4.56666666666667</v>
       </c>
-      <c r="E10" s="3" t="n">
-        <f aca="false">SUM(E3:E8)</f>
-        <v>214.866666666667</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <f aca="false">SUM(F3:F8)</f>
+      <c r="E11" s="6" t="n">
+        <f aca="false">SUM(E3:E9)</f>
+        <v>256.866666666667</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <f aca="false">SUM(F3:F9)</f>
         <v>247.166666666667</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="7" t="n">
-        <f aca="false">B10/8</f>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9" t="n">
+        <f aca="false">B11/8</f>
         <v>37.4166666666667</v>
       </c>
-      <c r="C11" s="7" t="n">
-        <f aca="false">C10/8</f>
+      <c r="C12" s="9" t="n">
+        <f aca="false">C11/8</f>
         <v>23.5</v>
       </c>
-      <c r="D11" s="7" t="n">
-        <f aca="false">D10/8</f>
-        <v>0.570833333333333</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">E10/8</f>
-        <v>26.8583333333333</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">F10/8</f>
+      <c r="D12" s="9" t="n">
+        <f aca="false">D11/8</f>
+        <v>0.570833333333334</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <f aca="false">E11/8</f>
+        <v>32.1083333333333</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <f aca="false">F11/8</f>
         <v>30.8958333333333</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <f aca="false">B11*4</f>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <f aca="false">B12*4</f>
         <v>149.666666666667</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="n">
-        <f aca="false">E11*9</f>
-        <v>241.725</v>
-      </c>
-      <c r="F13" s="3" t="n">
-        <f aca="false">F11*4</f>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="n">
+        <f aca="false">E12*9</f>
+        <v>288.975</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <f aca="false">F12*4</f>
         <v>123.583333333333</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3" t="n">
-        <f aca="false">B13+E13+F13</f>
-        <v>514.975</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <f aca="false">B14+E14+F14</f>
+        <v>562.225</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="https://www.dillons.com/p/russet-potato/0000000004072"/>
-    <hyperlink ref="H3" r:id="rId2" display="https://www.nutritionix.com/food/russet-potato"/>
-    <hyperlink ref="G4" r:id="rId3" display="https://www.dillons.com/p/simple-truth-natural-cage-free-large-brown-eggs/0001111079770"/>
-    <hyperlink ref="G5" r:id="rId4" display="https://www.dillons.com/p/kroger-diced-green-chile-peppers/0001111084009"/>
-    <hyperlink ref="G6" r:id="rId5" display="https://www.dillons.com/p/kroger-original-breakfast-sausage-links/0001111097293"/>
-    <hyperlink ref="G7" r:id="rId6" display="https://www.dillons.com/p/mission-carb-balance-low-carb-whole-wheat-burrito-tortillas/0007373100118"/>
-    <hyperlink ref="G8" r:id="rId7" display="https://www.dillons.com/p/kroger-shredded-mexican-style-cheese-blend/0001111050204"/>
+    <hyperlink ref="G3" r:id="rId1" display="https://www.dillons.com/p/simple-truth-organic-refined-avocado-oil-bottle/0001111003441"/>
+    <hyperlink ref="G4" r:id="rId2" display="https://www.dillons.com/p/russet-potato/0000000004072"/>
+    <hyperlink ref="H4" r:id="rId3" display="https://www.nutritionix.com/food/russet-potato"/>
+    <hyperlink ref="G5" r:id="rId4" display="https://www.dillons.com/p/simple-truth-natural-cage-free-large-brown-eggs/0001111079770"/>
+    <hyperlink ref="G6" r:id="rId5" display="https://www.dillons.com/p/kroger-diced-green-chile-peppers/0001111084009"/>
+    <hyperlink ref="G7" r:id="rId6" display="https://www.dillons.com/p/kroger-original-breakfast-sausage-links/0001111097293"/>
+    <hyperlink ref="G8" r:id="rId7" display="https://www.dillons.com/p/mission-carb-balance-low-carb-whole-wheat-burrito-tortillas/0007373100118"/>
+    <hyperlink ref="G9" r:id="rId8" display="https://www.dillons.com/p/kroger-shredded-mexican-style-cheese-blend/0001111050204"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
created python script for nutrition calculations
</commit_message>
<xml_diff>
--- a/nutrition-calcs/breakfast-burritos.xlsx
+++ b/nutrition-calcs/breakfast-burritos.xlsx
@@ -242,7 +242,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -561,14 +561,13 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="https://www.dillons.com/p/simple-truth-organic-refined-avocado-oil-bottle/0001111003441"/>
-    <hyperlink ref="G4" r:id="rId2" display="https://www.dillons.com/p/russet-potato/0000000004072"/>
-    <hyperlink ref="H4" r:id="rId3" display="https://www.nutritionix.com/food/russet-potato"/>
-    <hyperlink ref="G5" r:id="rId4" display="https://www.dillons.com/p/simple-truth-natural-cage-free-large-brown-eggs/0001111079770"/>
-    <hyperlink ref="G6" r:id="rId5" display="https://www.dillons.com/p/kroger-diced-green-chile-peppers/0001111084009"/>
-    <hyperlink ref="G7" r:id="rId6" display="https://www.dillons.com/p/kroger-original-breakfast-sausage-links/0001111097293"/>
-    <hyperlink ref="G8" r:id="rId7" display="https://www.dillons.com/p/mission-carb-balance-low-carb-whole-wheat-burrito-tortillas/0007373100118"/>
-    <hyperlink ref="G9" r:id="rId8" display="https://www.dillons.com/p/kroger-shredded-mexican-style-cheese-blend/0001111050204"/>
+    <hyperlink ref="G4" r:id="rId1" display="https://www.dillons.com/p/russet-potato/0000000004072"/>
+    <hyperlink ref="H4" r:id="rId2" display="https://www.nutritionix.com/food/russet-potato"/>
+    <hyperlink ref="G5" r:id="rId3" display="https://www.dillons.com/p/simple-truth-natural-cage-free-large-brown-eggs/0001111079770"/>
+    <hyperlink ref="G6" r:id="rId4" display="https://www.dillons.com/p/kroger-diced-green-chile-peppers/0001111084009"/>
+    <hyperlink ref="G7" r:id="rId5" display="https://www.dillons.com/p/kroger-original-breakfast-sausage-links/0001111097293"/>
+    <hyperlink ref="G8" r:id="rId6" display="https://www.dillons.com/p/mission-carb-balance-low-carb-whole-wheat-burrito-tortillas/0007373100118"/>
+    <hyperlink ref="G9" r:id="rId7" display="https://www.dillons.com/p/kroger-shredded-mexican-style-cheese-blend/0001111050204"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>